<commit_message>
Update Job allocation completion status
</commit_message>
<xml_diff>
--- a/Job_Allocation.xlsx
+++ b/Job_Allocation.xlsx
@@ -71,9 +71,6 @@
     <t xml:space="preserve">Table </t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>Xia Minghong</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Jingyuan</t>
+  </si>
+  <si>
+    <t>Member</t>
   </si>
 </sst>
 </file>
@@ -407,140 +407,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>16</v>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>